<commit_message>
Final FIM March 2023
</commit_message>
<xml_diff>
--- a/results/03-2023/comparison-deflators-03-2023.xlsx
+++ b/results/03-2023/comparison-deflators-03-2023.xlsx
@@ -855,31 +855,31 @@
         <v>-0.0617</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1087</v>
+        <v>-0.0784</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0596</v>
+        <v>0.0017</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1348</v>
+        <v>-0.0419</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1347</v>
+        <v>-0.0414</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.127</v>
+        <v>-0.0628</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0588</v>
+        <v>-0.024</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0216</v>
+        <v>0.0267</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0255</v>
+        <v>0.0308</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0356</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="8">
@@ -911,31 +911,31 @@
         <v>-0.4387</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1203</v>
+        <v>-0.1448</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0421</v>
+        <v>0.0079</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0943</v>
+        <v>0.0625</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1518</v>
+        <v>0.1251</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4239</v>
+        <v>0.4023</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4186</v>
+        <v>0.3972</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4505</v>
+        <v>0.4294</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4032</v>
+        <v>0.3823</v>
       </c>
       <c r="R8" t="n">
-        <v>0.2887</v>
+        <v>0.2794</v>
       </c>
     </row>
     <row r="9">
@@ -1359,31 +1359,31 @@
         <v>-0.9796</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.4652</v>
+        <v>-1.4594</v>
       </c>
       <c r="K16" t="n">
-        <v>-1.5877</v>
+        <v>-1.5607</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.5185</v>
+        <v>-0.4575</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.5489</v>
+        <v>-0.4824</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.5849</v>
+        <v>-0.5423</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.1673</v>
+        <v>-0.1539</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.097</v>
+        <v>-0.1131</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0442</v>
+        <v>0.0286</v>
       </c>
       <c r="R16" t="n">
-        <v>0.0103</v>
+        <v>0.0064</v>
       </c>
     </row>
     <row r="17">
@@ -2423,31 +2423,31 @@
         <v>-0.0008</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0007</v>
+        <v>0.031</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0097</v>
+        <v>0.0709</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0028</v>
+        <v>0.0956</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0039</v>
+        <v>0.0972</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0029</v>
+        <v>0.0671</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0053</v>
+        <v>0.0294</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0017</v>
+        <v>0.0068</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.0015</v>
+        <v>0.0068</v>
       </c>
       <c r="R35" t="n">
-        <v>0.0015</v>
+        <v>0.0069</v>
       </c>
     </row>
     <row r="36">
@@ -2479,31 +2479,31 @@
         <v>0.0024</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0024</v>
+        <v>-0.0222</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0012</v>
+        <v>-0.0331</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0012</v>
+        <v>-0.0307</v>
       </c>
       <c r="M36" t="n">
-        <v>0.0012</v>
+        <v>-0.0255</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0012</v>
+        <v>-0.0203</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0012</v>
+        <v>-0.0202</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0012</v>
+        <v>-0.02</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0001</v>
+        <v>-0.0209</v>
       </c>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>-0.0093</v>
       </c>
     </row>
     <row r="37">
@@ -2927,31 +2927,31 @@
         <v>0.0501</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0229</v>
+        <v>0.0287</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0184</v>
+        <v>0.0454</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0211</v>
+        <v>0.0821</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0134</v>
+        <v>0.08</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0119</v>
+        <v>0.0545</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0103</v>
+        <v>0.0236</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0085</v>
+        <v>-0.0076</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.0014</v>
+        <v>-0.0143</v>
       </c>
       <c r="R44" t="n">
-        <v>0.0014</v>
+        <v>-0.0025</v>
       </c>
     </row>
     <row r="45">

</xml_diff>